<commit_message>
modify aug pc result
</commit_message>
<xml_diff>
--- a/aug_pc_result/2026_Jan_21_11_32_30_d_separation_kci_pc_gt_graph_AdaSyn_20_909088/ori_pc_raw_eval_res.xlsx
+++ b/aug_pc_result/2026_Jan_21_11_32_30_d_separation_kci_pc_gt_graph_AdaSyn_20_909088/ori_pc_raw_eval_res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CausalLearning\code\aug_pc_result\2026_Jan_21_11_32_30_d_separation_kci_pc_gt_graph_AdaSyn_20_909088\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE5E299-B225-4845-A2E8-3C84CB8BD3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6276AF3-BE1E-4EF3-B24A-AF593894356A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -514,7 +514,7 @@
   <dimension ref="A1:AD257"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F219" workbookViewId="0">
-      <selection activeCell="M230" sqref="M230"/>
+      <selection activeCell="Q233" sqref="Q233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>

</xml_diff>